<commit_message>
fix kbv report table
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2022-05-01.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2022-05-01.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="427">
   <si>
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
@@ -160,12 +160,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gesamt Auffr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R0</t>
   </si>
   <si>
     <t xml:space="preserve">7-Tage-Inzidenz</t>
@@ -1757,22 +1751,22 @@
         <v>41</v>
       </c>
       <c r="B1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
         <v>323</v>
-      </c>
-      <c r="C1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="2">
@@ -1780,390 +1774,390 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D2" t="n">
         <v>440</v>
       </c>
       <c r="E2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F2" t="n">
         <v>711</v>
       </c>
       <c r="G2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D3" t="n">
         <v>433</v>
       </c>
       <c r="E3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F3" t="n">
         <v>661</v>
       </c>
       <c r="G3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D4" t="n">
         <v>466</v>
       </c>
       <c r="E4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F4" t="n">
         <v>744</v>
       </c>
       <c r="G4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D5" t="n">
         <v>300</v>
       </c>
       <c r="E5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F5" t="n">
         <v>539</v>
       </c>
       <c r="G5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D6" t="n">
         <v>376</v>
       </c>
       <c r="E6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F6" t="n">
         <v>559</v>
       </c>
       <c r="G6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D7" t="n">
         <v>436</v>
       </c>
       <c r="E7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F7" t="n">
         <v>698</v>
       </c>
       <c r="G7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D8" t="n">
         <v>525</v>
       </c>
       <c r="E8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F8" t="n">
         <v>942</v>
       </c>
       <c r="G8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D9" t="n">
         <v>522</v>
       </c>
       <c r="E9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F9" t="n">
         <v>831</v>
       </c>
       <c r="G9" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D10" t="n">
         <v>354</v>
       </c>
       <c r="E10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F10" t="n">
         <v>486</v>
       </c>
       <c r="G10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C11" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D11" t="n">
         <v>591</v>
       </c>
       <c r="E11" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F11" t="n">
         <v>1013</v>
       </c>
       <c r="G11" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C12" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D12" t="n">
         <v>411</v>
       </c>
       <c r="E12" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F12" t="n">
         <v>639</v>
       </c>
       <c r="G12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D13" t="n">
         <v>428</v>
       </c>
       <c r="E13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F13" t="n">
         <v>713</v>
       </c>
       <c r="G13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C14" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D14" t="n">
         <v>505</v>
       </c>
       <c r="E14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F14" t="n">
         <v>738</v>
       </c>
       <c r="G14" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D15" t="n">
         <v>365</v>
       </c>
       <c r="E15" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F15" t="n">
         <v>525</v>
       </c>
       <c r="G15" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C16" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D16" t="n">
         <v>377</v>
       </c>
       <c r="E16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F16" t="n">
         <v>578</v>
       </c>
       <c r="G16" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C17" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D17" t="n">
         <v>472</v>
       </c>
       <c r="E17" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F17" t="n">
         <v>991</v>
       </c>
       <c r="G17" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C18" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D18" t="n">
         <v>286</v>
       </c>
       <c r="E18" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F18" t="n">
         <v>424</v>
       </c>
       <c r="G18" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2182,354 +2176,354 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" t="s">
         <v>382</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>383</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>384</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>385</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>386</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>387</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>388</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>389</v>
-      </c>
-      <c r="I1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J1" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C2" t="n">
         <v>8228081</v>
       </c>
       <c r="D2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F2" t="n">
         <v>116059</v>
       </c>
       <c r="G2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H2" t="n">
         <v>1648</v>
       </c>
       <c r="I2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B3" t="s">
         <v>397</v>
-      </c>
-      <c r="B3" t="s">
-        <v>399</v>
       </c>
       <c r="C3" t="n">
         <v>4144906</v>
       </c>
       <c r="D3" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F3" t="n">
         <v>40164</v>
       </c>
       <c r="G3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H3" t="n">
         <v>1400</v>
       </c>
       <c r="I3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C4" t="n">
         <v>28872621</v>
       </c>
       <c r="D4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F4" t="n">
         <v>163612</v>
       </c>
       <c r="G4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H4" t="n">
         <v>1309</v>
       </c>
       <c r="I4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="J4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C5" t="n">
         <v>3906098</v>
       </c>
       <c r="D5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F5" t="n">
         <v>104462</v>
       </c>
       <c r="G5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H5" t="n">
         <v>1024</v>
       </c>
       <c r="I5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C6" t="n">
         <v>4056448</v>
       </c>
       <c r="D6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F6" t="n">
         <v>175552</v>
       </c>
       <c r="G6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H6" t="n">
         <v>723</v>
       </c>
       <c r="I6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="J6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C7" t="n">
         <v>22214004</v>
       </c>
       <c r="D7" t="s">
+        <v>410</v>
+      </c>
+      <c r="E7" t="s">
         <v>412</v>
-      </c>
-      <c r="E7" t="s">
-        <v>414</v>
       </c>
       <c r="F7" t="n">
         <v>31439</v>
       </c>
       <c r="G7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H7" t="n">
         <v>501</v>
       </c>
       <c r="I7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C8" t="n">
         <v>24813817</v>
       </c>
       <c r="D8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F8" t="n">
         <v>135461</v>
       </c>
       <c r="G8" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H8" t="n">
         <v>440</v>
       </c>
       <c r="I8" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="J8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C9" t="n">
         <v>16504791</v>
       </c>
       <c r="D9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F9" t="n">
         <v>146999</v>
       </c>
       <c r="G9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H9" t="n">
         <v>222</v>
       </c>
       <c r="I9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B10" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C10" t="n">
         <v>11896152</v>
       </c>
       <c r="D10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E10" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F10" t="n">
         <v>18161</v>
       </c>
       <c r="G10" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H10" t="n">
         <v>194</v>
       </c>
       <c r="I10" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C11" t="n">
         <v>5996748</v>
       </c>
       <c r="D11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F11" t="n">
         <v>22870</v>
       </c>
       <c r="G11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H11" t="n">
         <v>30</v>
       </c>
       <c r="I11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -2652,12 +2646,6 @@
       <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -2667,488 +2655,386 @@
         <v>438386</v>
       </c>
       <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" t="n">
-        <v>25214749</v>
+        <v>711</v>
       </c>
       <c r="G2" t="n">
-        <v>0.835635608156743</v>
-      </c>
-      <c r="H2" t="n">
-        <v>711</v>
-      </c>
-      <c r="I2" t="n">
         <v>440</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="n">
         <v>37245</v>
       </c>
       <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
       <c r="F3" t="n">
-        <v>3538834</v>
+        <v>661</v>
       </c>
       <c r="G3" t="n">
-        <v>0.845097700469601</v>
-      </c>
-      <c r="H3" t="n">
-        <v>661</v>
-      </c>
-      <c r="I3" t="n">
         <v>433</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" t="n">
         <v>41500</v>
       </c>
       <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
       <c r="F4" t="n">
-        <v>4709499</v>
+        <v>744</v>
       </c>
       <c r="G4" t="n">
-        <v>0.902531105329903</v>
-      </c>
-      <c r="H4" t="n">
-        <v>744</v>
-      </c>
-      <c r="I4" t="n">
         <v>466</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n">
         <v>32199</v>
       </c>
       <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
         <v>62</v>
       </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" t="s">
-        <v>64</v>
-      </c>
       <c r="F5" t="n">
-        <v>1012152</v>
+        <v>539</v>
       </c>
       <c r="G5" t="n">
-        <v>0.915735031591338</v>
-      </c>
-      <c r="H5" t="n">
-        <v>539</v>
-      </c>
-      <c r="I5" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" t="n">
         <v>13409</v>
       </c>
       <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
         <v>66</v>
       </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s">
-        <v>68</v>
-      </c>
       <c r="F6" t="n">
-        <v>771291</v>
+        <v>559</v>
       </c>
       <c r="G6" t="n">
-        <v>0.849805868569664</v>
-      </c>
-      <c r="H6" t="n">
-        <v>559</v>
-      </c>
-      <c r="I6" t="n">
         <v>376</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" t="n">
         <v>3450</v>
       </c>
       <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
         <v>70</v>
       </c>
-      <c r="D7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
       <c r="F7" t="n">
-        <v>189872</v>
+        <v>698</v>
       </c>
       <c r="G7" t="n">
-        <v>0.771676906641925</v>
-      </c>
-      <c r="H7" t="n">
-        <v>698</v>
-      </c>
-      <c r="I7" t="n">
         <v>436</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" t="n">
         <v>17771</v>
       </c>
       <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" t="s">
-        <v>76</v>
-      </c>
       <c r="F8" t="n">
-        <v>554775</v>
+        <v>942</v>
       </c>
       <c r="G8" t="n">
-        <v>0.779724517878986</v>
-      </c>
-      <c r="H8" t="n">
-        <v>942</v>
-      </c>
-      <c r="I8" t="n">
         <v>525</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" t="n">
         <v>32340</v>
       </c>
       <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
         <v>78</v>
       </c>
-      <c r="D9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" t="s">
-        <v>80</v>
-      </c>
       <c r="F9" t="n">
-        <v>1760651</v>
+        <v>831</v>
       </c>
       <c r="G9" t="n">
-        <v>0.835856040783773</v>
-      </c>
-      <c r="H9" t="n">
-        <v>831</v>
-      </c>
-      <c r="I9" t="n">
         <v>522</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" t="n">
         <v>13580</v>
       </c>
       <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" t="s">
         <v>82</v>
       </c>
-      <c r="D10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" t="s">
-        <v>84</v>
-      </c>
       <c r="F10" t="n">
-        <v>472842</v>
+        <v>486</v>
       </c>
       <c r="G10" t="n">
-        <v>0.754916805883977</v>
-      </c>
-      <c r="H10" t="n">
-        <v>486</v>
-      </c>
-      <c r="I10" t="n">
         <v>354</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B11" t="n">
         <v>51266</v>
       </c>
       <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" t="s">
         <v>86</v>
       </c>
-      <c r="D11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" t="s">
-        <v>88</v>
-      </c>
       <c r="F11" t="n">
-        <v>2217665</v>
+        <v>1013</v>
       </c>
       <c r="G11" t="n">
-        <v>0.820811567084433</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1013</v>
-      </c>
-      <c r="I11" t="n">
         <v>591</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" t="n">
         <v>134597</v>
       </c>
       <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" t="s">
         <v>90</v>
       </c>
-      <c r="D12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" t="s">
-        <v>92</v>
-      </c>
       <c r="F12" t="n">
-        <v>5032762</v>
+        <v>639</v>
       </c>
       <c r="G12" t="n">
-        <v>0.824525799893428</v>
-      </c>
-      <c r="H12" t="n">
-        <v>639</v>
-      </c>
-      <c r="I12" t="n">
         <v>411</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" t="n">
         <v>24615</v>
       </c>
       <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" t="s">
         <v>94</v>
       </c>
-      <c r="D13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" t="s">
-        <v>96</v>
-      </c>
       <c r="F13" t="n">
-        <v>1096372</v>
+        <v>713</v>
       </c>
       <c r="G13" t="n">
-        <v>0.776743291618283</v>
-      </c>
-      <c r="H13" t="n">
-        <v>713</v>
-      </c>
-      <c r="I13" t="n">
         <v>428</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B14" t="n">
         <v>5078</v>
       </c>
       <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
         <v>98</v>
       </c>
-      <c r="D14" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14" t="s">
-        <v>100</v>
-      </c>
       <c r="F14" t="n">
-        <v>304833</v>
+        <v>738</v>
       </c>
       <c r="G14" t="n">
-        <v>0.808626242244866</v>
-      </c>
-      <c r="H14" t="n">
-        <v>738</v>
-      </c>
-      <c r="I14" t="n">
         <v>505</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B15" t="n">
         <v>12555</v>
       </c>
       <c r="C15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" t="s">
         <v>102</v>
       </c>
-      <c r="D15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15" t="s">
-        <v>104</v>
-      </c>
       <c r="F15" t="n">
-        <v>1479628</v>
+        <v>525</v>
       </c>
       <c r="G15" t="n">
-        <v>0.805712553435448</v>
-      </c>
-      <c r="H15" t="n">
-        <v>525</v>
-      </c>
-      <c r="I15" t="n">
         <v>365</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" t="n">
         <v>11365</v>
       </c>
       <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
         <v>106</v>
       </c>
-      <c r="D16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E16" t="s">
-        <v>108</v>
-      </c>
       <c r="F16" t="n">
-        <v>699493</v>
+        <v>578</v>
       </c>
       <c r="G16" t="n">
-        <v>0.788680586184466</v>
-      </c>
-      <c r="H16" t="n">
-        <v>578</v>
-      </c>
-      <c r="I16" t="n">
         <v>377</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
       </c>
       <c r="C17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" t="s">
         <v>110</v>
       </c>
-      <c r="D17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" t="s">
-        <v>112</v>
-      </c>
       <c r="F17" t="n">
-        <v>677009</v>
+        <v>991</v>
       </c>
       <c r="G17" t="n">
-        <v>0.850244351302807</v>
-      </c>
-      <c r="H17" t="n">
-        <v>991</v>
-      </c>
-      <c r="I17" t="n">
         <v>472</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B18" t="n">
         <v>7001</v>
       </c>
       <c r="C18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
         <v>114</v>
       </c>
-      <c r="D18" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" t="s">
-        <v>116</v>
-      </c>
       <c r="F18" t="n">
-        <v>697071</v>
+        <v>424</v>
       </c>
       <c r="G18" t="n">
-        <v>0.720709285211598</v>
-      </c>
-      <c r="H18" t="n">
-        <v>424</v>
-      </c>
-      <c r="I18" t="n">
         <v>286</v>
       </c>
     </row>
@@ -3168,343 +3054,343 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
         <v>119</v>
-      </c>
-      <c r="B2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
         <v>122</v>
-      </c>
-      <c r="B3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
         <v>125</v>
-      </c>
-      <c r="B4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" t="s">
         <v>128</v>
-      </c>
-      <c r="B5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
         <v>131</v>
-      </c>
-      <c r="B6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
         <v>134</v>
-      </c>
-      <c r="B7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" t="s">
         <v>137</v>
-      </c>
-      <c r="B8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" t="s">
         <v>150</v>
-      </c>
-      <c r="B14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" t="s">
         <v>162</v>
-      </c>
-      <c r="B20" t="s">
-        <v>163</v>
-      </c>
-      <c r="C20" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>173</v>
+      </c>
+      <c r="B26" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" t="s">
         <v>175</v>
-      </c>
-      <c r="B26" t="s">
-        <v>176</v>
-      </c>
-      <c r="C26" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C30" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C31" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3523,13 +3409,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
         <v>26</v>
@@ -3537,72 +3423,72 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" t="s">
         <v>190</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>191</v>
-      </c>
-      <c r="C2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" t="s">
         <v>194</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>195</v>
-      </c>
-      <c r="C3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" t="s">
         <v>198</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>199</v>
-      </c>
-      <c r="C4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
         <v>202</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>203</v>
-      </c>
-      <c r="C5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" t="s">
         <v>206</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>207</v>
-      </c>
-      <c r="C6" t="s">
-        <v>208</v>
-      </c>
-      <c r="D6" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3621,13 +3507,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
         <v>26</v>
@@ -3635,21 +3521,21 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" t="s">
         <v>211</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>212</v>
-      </c>
-      <c r="C2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -3660,102 +3546,102 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" t="s">
         <v>216</v>
-      </c>
-      <c r="C4" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" t="s">
         <v>219</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>220</v>
-      </c>
-      <c r="C5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" t="s">
         <v>223</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>224</v>
-      </c>
-      <c r="C6" t="s">
-        <v>225</v>
-      </c>
-      <c r="D6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" t="s">
         <v>227</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>228</v>
-      </c>
-      <c r="C7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D7" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" t="s">
         <v>231</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>232</v>
-      </c>
-      <c r="C8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D8" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" t="s">
         <v>235</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>236</v>
-      </c>
-      <c r="C9" t="s">
-        <v>237</v>
-      </c>
-      <c r="D9" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" t="s">
         <v>239</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>240</v>
-      </c>
-      <c r="C10" t="s">
-        <v>241</v>
-      </c>
-      <c r="D10" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -3766,27 +3652,27 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" t="s">
         <v>244</v>
-      </c>
-      <c r="C12" t="s">
-        <v>245</v>
-      </c>
-      <c r="D12" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" t="s">
         <v>247</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>248</v>
-      </c>
-      <c r="C13" t="s">
-        <v>249</v>
-      </c>
-      <c r="D13" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3805,13 +3691,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D1" t="s">
         <v>26</v>
@@ -3822,97 +3708,97 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" t="s">
         <v>253</v>
-      </c>
-      <c r="C2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" t="s">
         <v>256</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>257</v>
-      </c>
-      <c r="C3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" t="s">
         <v>260</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>261</v>
-      </c>
-      <c r="C4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D4" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" t="s">
         <v>264</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>265</v>
-      </c>
-      <c r="C5" t="s">
-        <v>266</v>
-      </c>
-      <c r="D5" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" t="s">
         <v>268</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>269</v>
-      </c>
-      <c r="C6" t="s">
-        <v>270</v>
-      </c>
-      <c r="D6" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" t="s">
         <v>272</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>273</v>
-      </c>
-      <c r="C7" t="s">
-        <v>274</v>
-      </c>
-      <c r="D7" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C8" t="s">
         <v>276</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>277</v>
-      </c>
-      <c r="C8" t="s">
-        <v>278</v>
-      </c>
-      <c r="D8" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -3931,13 +3817,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
         <v>26</v>
@@ -3945,44 +3831,44 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" t="s">
         <v>281</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>282</v>
-      </c>
-      <c r="C2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" t="s">
         <v>285</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>286</v>
-      </c>
-      <c r="C3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" t="s">
         <v>289</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>290</v>
-      </c>
-      <c r="C4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D4" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -4001,13 +3887,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D1" t="s">
         <v>26</v>
@@ -4015,44 +3901,44 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" t="s">
         <v>295</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>296</v>
-      </c>
-      <c r="C2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D2" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" t="s">
         <v>299</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>300</v>
-      </c>
-      <c r="C3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D3" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" t="s">
         <v>303</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>304</v>
-      </c>
-      <c r="C4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="5">
@@ -4060,18 +3946,18 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" t="s">
         <v>307</v>
-      </c>
-      <c r="C5" t="s">
-        <v>308</v>
-      </c>
-      <c r="D5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
@@ -4079,44 +3965,44 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C7" t="s">
+        <v>310</v>
+      </c>
+      <c r="D7" t="s">
         <v>311</v>
-      </c>
-      <c r="C7" t="s">
-        <v>312</v>
-      </c>
-      <c r="D7" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D8" t="s">
         <v>314</v>
-      </c>
-      <c r="C8" t="s">
-        <v>315</v>
-      </c>
-      <c r="D8" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" t="s">
         <v>317</v>
-      </c>
-      <c r="C9" t="s">
-        <v>318</v>
-      </c>
-      <c r="D9" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="10">
@@ -4124,13 +4010,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C10" t="s">
+        <v>319</v>
+      </c>
+      <c r="D10" t="s">
         <v>320</v>
-      </c>
-      <c r="C10" t="s">
-        <v>321</v>
-      </c>
-      <c r="D10" t="s">
-        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>